<commit_message>
Fixes #48 - ssmmessages and ec2messages are compliant when SSM is compliant. Also modified the scraping functions to allow you to toggle whether or not to download updated files
</commit_message>
<xml_diff>
--- a/aws_allowlister/data/compliance_statuses.xlsx
+++ b/aws_allowlister/data/compliance_statuses.xlsx
@@ -1371,7 +1371,9 @@
         <v>1</v>
       </c>
       <c r="I31" t="inlineStr"/>
-      <c r="J31" t="inlineStr"/>
+      <c r="J31" t="b">
+        <v>1</v>
+      </c>
       <c r="K31" t="b">
         <v>1</v>
       </c>
@@ -2131,7 +2133,9 @@
         <v>1</v>
       </c>
       <c r="I56" t="inlineStr"/>
-      <c r="J56" t="inlineStr"/>
+      <c r="J56" t="b">
+        <v>1</v>
+      </c>
       <c r="K56" t="b">
         <v>1</v>
       </c>
@@ -3146,16 +3150,34 @@
           <t>Amazon Message Delivery Service</t>
         </is>
       </c>
-      <c r="C90" t="inlineStr"/>
-      <c r="D90" t="inlineStr"/>
-      <c r="E90" t="inlineStr"/>
-      <c r="F90" t="inlineStr"/>
-      <c r="G90" t="inlineStr"/>
-      <c r="H90" t="inlineStr"/>
+      <c r="C90" t="b">
+        <v>1</v>
+      </c>
+      <c r="D90" t="b">
+        <v>1</v>
+      </c>
+      <c r="E90" t="b">
+        <v>1</v>
+      </c>
+      <c r="F90" t="b">
+        <v>1</v>
+      </c>
+      <c r="G90" t="b">
+        <v>1</v>
+      </c>
+      <c r="H90" t="b">
+        <v>1</v>
+      </c>
       <c r="I90" t="inlineStr"/>
-      <c r="J90" t="inlineStr"/>
-      <c r="K90" t="inlineStr"/>
-      <c r="L90" t="inlineStr"/>
+      <c r="J90" t="b">
+        <v>1</v>
+      </c>
+      <c r="K90" t="b">
+        <v>1</v>
+      </c>
+      <c r="L90" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -5351,7 +5373,9 @@
         <v>1</v>
       </c>
       <c r="I160" t="inlineStr"/>
-      <c r="J160" t="inlineStr"/>
+      <c r="J160" t="b">
+        <v>1</v>
+      </c>
       <c r="K160" t="inlineStr"/>
       <c r="L160" t="b">
         <v>1</v>
@@ -5387,7 +5411,9 @@
         <v>1</v>
       </c>
       <c r="I161" t="inlineStr"/>
-      <c r="J161" t="inlineStr"/>
+      <c r="J161" t="b">
+        <v>1</v>
+      </c>
       <c r="K161" t="inlineStr"/>
       <c r="L161" t="b">
         <v>1</v>
@@ -7478,16 +7504,34 @@
           <t>Amazon Session Manager Message Gateway Service</t>
         </is>
       </c>
-      <c r="C229" t="inlineStr"/>
-      <c r="D229" t="inlineStr"/>
-      <c r="E229" t="inlineStr"/>
-      <c r="F229" t="inlineStr"/>
-      <c r="G229" t="inlineStr"/>
-      <c r="H229" t="inlineStr"/>
+      <c r="C229" t="b">
+        <v>1</v>
+      </c>
+      <c r="D229" t="b">
+        <v>1</v>
+      </c>
+      <c r="E229" t="b">
+        <v>1</v>
+      </c>
+      <c r="F229" t="b">
+        <v>1</v>
+      </c>
+      <c r="G229" t="b">
+        <v>1</v>
+      </c>
+      <c r="H229" t="b">
+        <v>1</v>
+      </c>
       <c r="I229" t="inlineStr"/>
-      <c r="J229" t="inlineStr"/>
-      <c r="K229" t="inlineStr"/>
-      <c r="L229" t="inlineStr"/>
+      <c r="J229" t="b">
+        <v>1</v>
+      </c>
+      <c r="K229" t="b">
+        <v>1</v>
+      </c>
+      <c r="L229" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="230">
       <c r="A230" t="inlineStr">
@@ -8361,7 +8405,9 @@
         <v>1</v>
       </c>
       <c r="I256" t="inlineStr"/>
-      <c r="J256" t="inlineStr"/>
+      <c r="J256" t="b">
+        <v>1</v>
+      </c>
       <c r="K256" t="b">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Updated compliance_statuses and compliance.db
</commit_message>
<xml_diff>
--- a/aws_allowlister/data/compliance_statuses.xlsx
+++ b/aws_allowlister/data/compliance_statuses.xlsx
@@ -1577,9 +1577,7 @@
       <c r="E39" t="b">
         <v>1</v>
       </c>
-      <c r="F39" t="b">
-        <v>1</v>
-      </c>
+      <c r="F39" t="inlineStr"/>
       <c r="G39" t="b">
         <v>1</v>
       </c>
@@ -1719,9 +1717,7 @@
       <c r="E43" t="b">
         <v>1</v>
       </c>
-      <c r="F43" t="b">
-        <v>1</v>
-      </c>
+      <c r="F43" t="inlineStr"/>
       <c r="G43" t="b">
         <v>1</v>
       </c>
@@ -1759,7 +1755,9 @@
       <c r="E44" t="b">
         <v>1</v>
       </c>
-      <c r="F44" t="inlineStr"/>
+      <c r="F44" t="b">
+        <v>1</v>
+      </c>
       <c r="G44" t="inlineStr"/>
       <c r="H44" t="b">
         <v>1</v>
@@ -2235,9 +2233,7 @@
       <c r="E60" t="b">
         <v>1</v>
       </c>
-      <c r="F60" t="b">
-        <v>1</v>
-      </c>
+      <c r="F60" t="inlineStr"/>
       <c r="G60" t="b">
         <v>1</v>
       </c>
@@ -2275,9 +2271,7 @@
       <c r="E61" t="b">
         <v>1</v>
       </c>
-      <c r="F61" t="b">
-        <v>1</v>
-      </c>
+      <c r="F61" t="inlineStr"/>
       <c r="G61" t="b">
         <v>1</v>
       </c>
@@ -2315,9 +2309,7 @@
       <c r="E62" t="b">
         <v>1</v>
       </c>
-      <c r="F62" t="b">
-        <v>1</v>
-      </c>
+      <c r="F62" t="inlineStr"/>
       <c r="G62" t="b">
         <v>1</v>
       </c>
@@ -2491,9 +2483,7 @@
       <c r="E67" t="b">
         <v>1</v>
       </c>
-      <c r="F67" t="b">
-        <v>1</v>
-      </c>
+      <c r="F67" t="inlineStr"/>
       <c r="G67" t="b">
         <v>1</v>
       </c>
@@ -3301,9 +3291,7 @@
       <c r="E94" t="b">
         <v>1</v>
       </c>
-      <c r="F94" t="b">
-        <v>1</v>
-      </c>
+      <c r="F94" t="inlineStr"/>
       <c r="G94" t="b">
         <v>1</v>
       </c>
@@ -5363,9 +5351,7 @@
       <c r="E160" t="b">
         <v>1</v>
       </c>
-      <c r="F160" t="b">
-        <v>1</v>
-      </c>
+      <c r="F160" t="inlineStr"/>
       <c r="G160" t="b">
         <v>1</v>
       </c>
@@ -5401,9 +5387,7 @@
       <c r="E161" t="b">
         <v>1</v>
       </c>
-      <c r="F161" t="b">
-        <v>1</v>
-      </c>
+      <c r="F161" t="inlineStr"/>
       <c r="G161" t="b">
         <v>1</v>
       </c>
@@ -5763,9 +5747,7 @@
       <c r="E175" t="b">
         <v>1</v>
       </c>
-      <c r="F175" t="b">
-        <v>1</v>
-      </c>
+      <c r="F175" t="inlineStr"/>
       <c r="G175" t="b">
         <v>1</v>
       </c>
@@ -6317,9 +6299,7 @@
       <c r="E194" t="b">
         <v>1</v>
       </c>
-      <c r="F194" t="b">
-        <v>1</v>
-      </c>
+      <c r="F194" t="inlineStr"/>
       <c r="G194" t="b">
         <v>1</v>
       </c>
@@ -7011,9 +6991,7 @@
       <c r="E215" t="b">
         <v>1</v>
       </c>
-      <c r="F215" t="b">
-        <v>1</v>
-      </c>
+      <c r="F215" t="inlineStr"/>
       <c r="G215" t="b">
         <v>1</v>
       </c>
@@ -7179,9 +7157,7 @@
       <c r="E220" t="b">
         <v>1</v>
       </c>
-      <c r="F220" t="b">
-        <v>1</v>
-      </c>
+      <c r="F220" t="inlineStr"/>
       <c r="G220" t="b">
         <v>1</v>
       </c>
@@ -7217,9 +7193,7 @@
       <c r="E221" t="b">
         <v>1</v>
       </c>
-      <c r="F221" t="b">
-        <v>1</v>
-      </c>
+      <c r="F221" t="inlineStr"/>
       <c r="G221" t="b">
         <v>1</v>
       </c>
@@ -7319,9 +7293,7 @@
       <c r="E224" t="b">
         <v>1</v>
       </c>
-      <c r="F224" t="b">
-        <v>1</v>
-      </c>
+      <c r="F224" t="inlineStr"/>
       <c r="G224" t="b">
         <v>1</v>
       </c>
@@ -7641,7 +7613,9 @@
       <c r="E233" t="b">
         <v>1</v>
       </c>
-      <c r="F233" t="inlineStr"/>
+      <c r="F233" t="b">
+        <v>1</v>
+      </c>
       <c r="G233" t="inlineStr"/>
       <c r="H233" t="b">
         <v>1</v>
@@ -8237,9 +8211,7 @@
       <c r="E251" t="b">
         <v>1</v>
       </c>
-      <c r="F251" t="b">
-        <v>1</v>
-      </c>
+      <c r="F251" t="inlineStr"/>
       <c r="G251" t="b">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Changes to makefile to update with latest compliance data; added examle AWS Commercial-only SCP
</commit_message>
<xml_diff>
--- a/aws_allowlister/data/compliance_statuses.xlsx
+++ b/aws_allowlister/data/compliance_statuses.xlsx
@@ -555,10 +555,16 @@
         </is>
       </c>
       <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
+      <c r="D3" t="b">
+        <v>1</v>
+      </c>
       <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
+      <c r="F3" t="b">
+        <v>1</v>
+      </c>
+      <c r="G3" t="b">
+        <v>1</v>
+      </c>
       <c r="H3" t="inlineStr"/>
       <c r="I3" t="inlineStr"/>
       <c r="J3" t="inlineStr"/>
@@ -653,8 +659,12 @@
       <c r="I5" t="b">
         <v>1</v>
       </c>
-      <c r="J5" t="inlineStr"/>
-      <c r="K5" t="inlineStr"/>
+      <c r="J5" t="b">
+        <v>1</v>
+      </c>
+      <c r="K5" t="b">
+        <v>1</v>
+      </c>
       <c r="L5" t="b">
         <v>1</v>
       </c>
@@ -1647,8 +1657,12 @@
       <c r="I33" t="b">
         <v>1</v>
       </c>
-      <c r="J33" t="inlineStr"/>
-      <c r="K33" t="inlineStr"/>
+      <c r="J33" t="b">
+        <v>1</v>
+      </c>
+      <c r="K33" t="b">
+        <v>1</v>
+      </c>
       <c r="L33" t="b">
         <v>1</v>
       </c>
@@ -9211,8 +9225,12 @@
       <c r="I233" t="b">
         <v>1</v>
       </c>
-      <c r="J233" t="inlineStr"/>
-      <c r="K233" t="inlineStr"/>
+      <c r="J233" t="b">
+        <v>1</v>
+      </c>
+      <c r="K233" t="b">
+        <v>1</v>
+      </c>
       <c r="L233" t="b">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Fix backup-storage in a new version
</commit_message>
<xml_diff>
--- a/aws_allowlister/data/compliance_statuses.xlsx
+++ b/aws_allowlister/data/compliance_statuses.xlsx
@@ -1610,20 +1610,34 @@
           <t>AWS Backup storage</t>
         </is>
       </c>
-      <c r="C32" t="inlineStr"/>
-      <c r="D32" t="inlineStr"/>
-      <c r="E32" t="inlineStr"/>
+      <c r="C32" t="b">
+        <v>1</v>
+      </c>
+      <c r="D32" t="b">
+        <v>1</v>
+      </c>
+      <c r="E32" t="b">
+        <v>1</v>
+      </c>
       <c r="F32" t="inlineStr"/>
       <c r="G32" t="inlineStr"/>
       <c r="H32" t="inlineStr"/>
       <c r="I32" t="inlineStr"/>
       <c r="J32" t="inlineStr"/>
       <c r="K32" t="inlineStr"/>
-      <c r="L32" t="inlineStr"/>
+      <c r="L32" t="b">
+        <v>1</v>
+      </c>
       <c r="M32" t="inlineStr"/>
-      <c r="N32" t="inlineStr"/>
-      <c r="O32" t="inlineStr"/>
-      <c r="P32" t="inlineStr"/>
+      <c r="N32" t="b">
+        <v>1</v>
+      </c>
+      <c r="O32" t="b">
+        <v>1</v>
+      </c>
+      <c r="P32" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">

</xml_diff>